<commit_message>
updated excel reference output
</commit_message>
<xml_diff>
--- a/tests/analyzer/reference_calculations.xlsx
+++ b/tests/analyzer/reference_calculations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BenjaminYe\Projects\portana\tests\analyzer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5CC07B3-96E2-4A1D-B37A-20DFF7D594F6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C29D3F47-3560-4776-BAD2-E7D5C7D2D278}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22305" yWindow="14340" windowWidth="21645" windowHeight="13935" xr2:uid="{13B1BA99-2CC8-48E1-ADFD-55A06DB185AD}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="13">
   <si>
     <t>Security 1</t>
   </si>
@@ -64,15 +64,25 @@
   </si>
   <si>
     <t>Drawdowns</t>
+  </si>
+  <si>
+    <t>Max Drawdowns</t>
+  </si>
+  <si>
+    <t>Max Drawdown Dates</t>
+  </si>
+  <si>
+    <t>Helpers</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.00000"/>
     <numFmt numFmtId="165" formatCode="0.000000"/>
+    <numFmt numFmtId="167" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -91,12 +101,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -120,7 +136,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -132,6 +148,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -446,21 +466,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D25D53C3-D339-4000-B5D5-6F97F46D2A71}">
-  <dimension ref="B2:N32"/>
+  <dimension ref="B2:N38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="H45" sqref="H45"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="I45" sqref="I45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.7109375" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="5" width="12.7109375" customWidth="1"/>
-    <col min="7" max="7" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="10" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
@@ -485,9 +506,14 @@
       <c r="J2" s="4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B3" s="1">
+      <c r="L2" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="M2" s="7"/>
+      <c r="N2" s="7"/>
+    </row>
+    <row r="3" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B3" s="8">
         <v>43831</v>
       </c>
       <c r="C3" s="3">
@@ -515,8 +541,8 @@
         <v>1.0000000000000009E-2</v>
       </c>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B4" s="1">
+    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B4" s="8">
         <f>B3+1</f>
         <v>43832</v>
       </c>
@@ -545,8 +571,8 @@
         <v>9.9009900990099098E-3</v>
       </c>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B5" s="1">
+    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B5" s="8">
         <f t="shared" ref="B5:B8" si="4">B4+1</f>
         <v>43833</v>
       </c>
@@ -575,8 +601,8 @@
         <v>9.8039215686274161E-3</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B6" s="1">
+    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B6" s="8">
         <f t="shared" si="4"/>
         <v>43834</v>
       </c>
@@ -605,8 +631,8 @@
         <v>-9.7087378640776656E-3</v>
       </c>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B7" s="1">
+    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B7" s="8">
         <f t="shared" si="4"/>
         <v>43835</v>
       </c>
@@ -635,8 +661,8 @@
         <v>2.9411764705882248E-2</v>
       </c>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B8" s="1">
+    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B8" s="8">
         <f t="shared" si="4"/>
         <v>43836</v>
       </c>
@@ -650,7 +676,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
       <c r="G9" s="2" t="s">
         <v>5</v>
       </c>
@@ -664,8 +690,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="G10" s="1">
+    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="G10" s="8">
         <v>43831</v>
       </c>
       <c r="H10">
@@ -678,8 +704,8 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="G11" s="1">
+    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="G11" s="8">
         <f>G10+1</f>
         <v>43832</v>
       </c>
@@ -696,8 +722,8 @@
         <v>1010</v>
       </c>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="G12" s="1">
+    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="G12" s="8">
         <f t="shared" ref="G12:G15" si="6">G11+1</f>
         <v>43833</v>
       </c>
@@ -714,8 +740,8 @@
         <v>1020</v>
       </c>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="G13" s="1">
+    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="G13" s="8">
         <f t="shared" si="6"/>
         <v>43834</v>
       </c>
@@ -732,8 +758,8 @@
         <v>1030</v>
       </c>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="G14" s="1">
+    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="G14" s="8">
         <f t="shared" si="6"/>
         <v>43835</v>
       </c>
@@ -750,8 +776,8 @@
         <v>1020</v>
       </c>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="G15" s="1">
+    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="G15" s="8">
         <f t="shared" si="6"/>
         <v>43836</v>
       </c>
@@ -783,7 +809,7 @@
       </c>
     </row>
     <row r="18" spans="7:14" x14ac:dyDescent="0.25">
-      <c r="G18" s="1">
+      <c r="G18" s="8">
         <v>43836</v>
       </c>
       <c r="H18" s="6">
@@ -814,7 +840,7 @@
       </c>
     </row>
     <row r="21" spans="7:14" x14ac:dyDescent="0.25">
-      <c r="G21" s="1">
+      <c r="G21" s="8">
         <v>43836</v>
       </c>
       <c r="H21" s="6">
@@ -845,7 +871,7 @@
       </c>
     </row>
     <row r="24" spans="7:14" x14ac:dyDescent="0.25">
-      <c r="G24" s="1">
+      <c r="G24" s="8">
         <v>43836</v>
       </c>
       <c r="H24">
@@ -876,7 +902,7 @@
       </c>
     </row>
     <row r="27" spans="7:14" x14ac:dyDescent="0.25">
-      <c r="G27" s="1">
+      <c r="G27" s="8">
         <v>43831</v>
       </c>
       <c r="H27">
@@ -905,7 +931,7 @@
       </c>
     </row>
     <row r="28" spans="7:14" x14ac:dyDescent="0.25">
-      <c r="G28" s="1">
+      <c r="G28" s="8">
         <f>G27+1</f>
         <v>43832</v>
       </c>
@@ -935,7 +961,7 @@
       </c>
     </row>
     <row r="29" spans="7:14" x14ac:dyDescent="0.25">
-      <c r="G29" s="1">
+      <c r="G29" s="8">
         <f t="shared" ref="G29:G32" si="17">G28+1</f>
         <v>43833</v>
       </c>
@@ -965,7 +991,7 @@
       </c>
     </row>
     <row r="30" spans="7:14" x14ac:dyDescent="0.25">
-      <c r="G30" s="1">
+      <c r="G30" s="8">
         <f t="shared" si="17"/>
         <v>43834</v>
       </c>
@@ -995,7 +1021,7 @@
       </c>
     </row>
     <row r="31" spans="7:14" x14ac:dyDescent="0.25">
-      <c r="G31" s="1">
+      <c r="G31" s="8">
         <f t="shared" si="17"/>
         <v>43835</v>
       </c>
@@ -1025,7 +1051,7 @@
       </c>
     </row>
     <row r="32" spans="7:14" x14ac:dyDescent="0.25">
-      <c r="G32" s="1">
+      <c r="G32" s="8">
         <f t="shared" si="17"/>
         <v>43836</v>
       </c>
@@ -1052,6 +1078,80 @@
       <c r="N32">
         <f>MAX(E$3:E8)</f>
         <v>105</v>
+      </c>
+    </row>
+    <row r="34" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="G34" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H34" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="I34" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="J34" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="G35" s="8">
+        <v>43836</v>
+      </c>
+      <c r="H35">
+        <f>MIN(H27:H32)</f>
+        <v>0</v>
+      </c>
+      <c r="I35">
+        <f t="shared" ref="I35:J35" si="18">MIN(I27:I32)</f>
+        <v>-0.03</v>
+      </c>
+      <c r="J35">
+        <f t="shared" si="18"/>
+        <v>-9.7087378640776691E-3</v>
+      </c>
+    </row>
+    <row r="37" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="G37" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H37" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="I37" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="J37" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="G38" s="8">
+        <v>43836</v>
+      </c>
+      <c r="H38" s="8">
+        <f ca="1">OFFSET($G$26,L38,0)</f>
+        <v>43831</v>
+      </c>
+      <c r="I38" s="8">
+        <f t="shared" ref="I38:J38" ca="1" si="19">OFFSET($G$26,M38,0)</f>
+        <v>43833</v>
+      </c>
+      <c r="J38" s="8">
+        <f t="shared" ca="1" si="19"/>
+        <v>43835</v>
+      </c>
+      <c r="L38">
+        <f>MATCH(H35,H27:H32,0)</f>
+        <v>1</v>
+      </c>
+      <c r="M38">
+        <f t="shared" ref="M38:N38" si="20">MATCH(I35,I27:I32,0)</f>
+        <v>3</v>
+      </c>
+      <c r="N38">
+        <f t="shared" si="20"/>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>